<commit_message>
Ads hydrogen to the model (production and UGS)
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_FossilELC.xlsx
+++ b/SubRes_Tmpl/SubRES_FossilELC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IEMM\IEMM_MIG\IEMM_VEDA_MIG_Template\SubRes_Tmpl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\Veda_models\IEMM_v60_10-1-master\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475B0DB6-539B-44B7-A12C-B091D80F2540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F2732C-C0FD-475A-BCCF-E67ED46DB093}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9435" yWindow="-17400" windowWidth="30960" windowHeight="16920" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="27" r:id="rId1"/>
@@ -22,7 +22,18 @@
     <sheet name="ELC_CO2 Transport and Storage" sheetId="20" r:id="rId7"/>
     <sheet name="ELC_Storage" sheetId="19" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -63,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="159">
   <si>
     <t>TechName</t>
   </si>
@@ -534,6 +545,12 @@
   </si>
   <si>
     <t>Creates the available new fossil power plants, CCS storage placeholder infrastructure and battery storage</t>
+  </si>
+  <si>
+    <t>EN_STG_PHS</t>
+  </si>
+  <si>
+    <t>Pumped hydro storage</t>
   </si>
 </sst>
 </file>
@@ -541,12 +558,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="166" formatCode="m\o\n\th\ d\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="#.00"/>
-    <numFmt numFmtId="168" formatCode="#."/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="167" formatCode="m\o\n\th\ d\,\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="#.00"/>
+    <numFmt numFmtId="169" formatCode="#."/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -878,11 +895,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -898,10 +915,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -929,7 +946,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -943,11 +960,11 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="16"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -991,11 +1008,11 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="31">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Comma 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Date" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Entrée" xfId="13" builtinId="20"/>
     <cellStyle name="Fixed" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Footnotes: all except top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -1004,7 +1021,7 @@
     <cellStyle name="Header: top rows" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Heading1" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Heading2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Input" xfId="13" builtinId="20"/>
+    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Normal 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
@@ -1015,9 +1032,9 @@
     <cellStyle name="Normal_Sheet1" xfId="27" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Normal_Sheet2" xfId="29" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Parent row" xfId="19" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Percent" xfId="20" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="Percent 3" xfId="22" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Pourcentage" xfId="20" builtinId="5"/>
     <cellStyle name="Section Break" xfId="23" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Section Break: parent row" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="Standard_WEO 2008 - RE Technology Cost (status 27-03-2008)-ext" xfId="25" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
@@ -1042,7 +1059,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1368,7 +1385,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="23" t="s">
@@ -1423,7 +1440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="36" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="36"/>
@@ -1456,7 +1473,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -5236,7 +5253,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
@@ -8955,7 +8972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="16" t="s">
@@ -11390,7 +11407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
@@ -13824,7 +13841,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
@@ -14132,13 +14149,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:Q20"/>
+  <dimension ref="B2:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -14156,12 +14173,12 @@
     <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17">
+    <row r="2" spans="2:18">
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:17">
+    <row r="3" spans="2:18">
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -14184,7 +14201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:17">
+    <row r="4" spans="2:18">
       <c r="B4" s="9" t="s">
         <v>71</v>
       </c>
@@ -14205,7 +14222,7 @@
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="2:17">
+    <row r="5" spans="2:18">
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
@@ -14226,19 +14243,34 @@
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="2:17">
-      <c r="B6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="8" spans="2:17" s="12" customFormat="1">
+    <row r="6" spans="2:18">
+      <c r="B6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="8" spans="2:18" s="12" customFormat="1">
       <c r="D8" s="36"/>
       <c r="G8" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:17">
+    <row r="9" spans="2:18">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -14288,7 +14320,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="2:17">
+    <row r="10" spans="2:18">
       <c r="B10" t="s">
         <v>140</v>
       </c>
@@ -14322,7 +14354,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="11" spans="2:17">
+    <row r="11" spans="2:18">
       <c r="D11" s="13"/>
       <c r="F11" t="s">
         <v>151</v>
@@ -14338,10 +14370,10 @@
       </c>
       <c r="N11" s="36"/>
     </row>
-    <row r="12" spans="2:17" s="36" customFormat="1">
+    <row r="12" spans="2:18" s="36" customFormat="1">
       <c r="D12" s="13"/>
       <c r="F12" s="13" t="str">
-        <f>C19</f>
+        <f>C25</f>
         <v>AuxStoIN</v>
       </c>
       <c r="G12" s="36" t="s">
@@ -14352,7 +14384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:17" s="12" customFormat="1">
+    <row r="13" spans="2:18" s="12" customFormat="1">
       <c r="B13" t="s">
         <v>93</v>
       </c>
@@ -14373,76 +14405,166 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:17" s="12" customFormat="1">
+    <row r="14" spans="2:18" s="12" customFormat="1">
+      <c r="B14" s="13" t="str">
+        <f>C6</f>
+        <v>EN_STG_PHS</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="36"/>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="9" t="s">
+      <c r="E14" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="36">
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="34">
+        <v>29.891943130000001</v>
+      </c>
+      <c r="J14" s="36">
+        <v>1</v>
+      </c>
+      <c r="K14" s="36">
+        <v>1200</v>
+      </c>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36">
+        <v>50</v>
+      </c>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36">
+        <v>17</v>
+      </c>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="36" t="str">
+        <f>F15</f>
+        <v>AuxStoOUT</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="34">
+        <f>1/H14</f>
+        <v>1.25</v>
+      </c>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="13" t="str">
+        <f>C25</f>
+        <v>AuxStoIN</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="36"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="9" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="9" t="s">
+    <row r="25" spans="2:9">
+      <c r="B25" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="C20" s="13" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="C26" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D26" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="F26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding a new file for LCOE calculations
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_FossilELC.xlsx
+++ b/SubRes_Tmpl/SubRES_FossilELC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\Veda_models\IEMM_v60_10-1-master\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SubRes_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F2732C-C0FD-475A-BCCF-E67ED46DB093}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B0BD2-99CC-417F-A66C-8C54DAF6DDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9435" yWindow="-17400" windowWidth="30960" windowHeight="16920" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3672" yWindow="-17388" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="27" r:id="rId1"/>
@@ -558,12 +558,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="167" formatCode="m\o\n\th\ d\,\ yyyy"/>
-    <numFmt numFmtId="168" formatCode="#.00"/>
-    <numFmt numFmtId="169" formatCode="#."/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="166" formatCode="m\o\n\th\ d\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="#.00"/>
+    <numFmt numFmtId="168" formatCode="#."/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -895,11 +895,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -915,10 +915,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -960,11 +960,11 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="16"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1008,11 +1008,11 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="31">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Comma 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Date" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Entrée" xfId="13" builtinId="20"/>
     <cellStyle name="Fixed" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Footnotes: all except top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -1021,7 +1021,7 @@
     <cellStyle name="Header: top rows" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Heading1" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Heading2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
+    <cellStyle name="Input" xfId="13" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Normal 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
@@ -1032,9 +1032,9 @@
     <cellStyle name="Normal_Sheet1" xfId="27" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Normal_Sheet2" xfId="29" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Parent row" xfId="19" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Percent" xfId="20" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="Percent 3" xfId="22" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Pourcentage" xfId="20" builtinId="5"/>
     <cellStyle name="Section Break" xfId="23" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Section Break: parent row" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="Standard_WEO 2008 - RE Technology Cost (status 27-03-2008)-ext" xfId="25" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
@@ -1059,7 +1059,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1385,7 +1385,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="23" t="s">
@@ -1440,10 +1440,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="1" width="9.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1473,30 +1473,30 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="26" width="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="34" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5253,32 +5253,32 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="36" customWidth="1"/>
     <col min="5" max="5" width="7" style="36" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" style="36" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" style="36" bestFit="1" customWidth="1"/>
     <col min="21" max="26" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.6640625" style="36" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" style="36" bestFit="1" customWidth="1"/>
     <col min="31" max="34" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="36"/>
+    <col min="35" max="16384" width="9.109375" style="36"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:30">
@@ -8972,7 +8972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="16" t="s">
@@ -9053,7 +9053,7 @@
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
     </row>
-    <row r="4" spans="1:23" ht="45">
+    <row r="4" spans="1:23" ht="43.2">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -11407,7 +11407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="16" t="s">
@@ -11453,7 +11453,7 @@
         <v>3.4123222748815167</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="45">
+    <row r="4" spans="1:20" ht="43.2">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -13841,26 +13841,26 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
@@ -14152,25 +14152,26 @@
   <dimension ref="B2:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+      <selection activeCell="B14" sqref="B14:R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18">

</xml_diff>